<commit_message>
analises de algoritmo oneR e prism
</commit_message>
<xml_diff>
--- a/machine-learning/dataset/tabelas_risco_credito_probabilidade_naive_bayes.xlsx
+++ b/machine-learning/dataset/tabelas_risco_credito_probabilidade_naive_bayes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\estudo-machine-learning\estudo-python\machine-learning\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E2112F-639F-471B-880C-5043D18619E1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52BF14DD-2A4F-48D4-838A-38CA606AE7E0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="513" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="513" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabela_credito_historica" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="88">
   <si>
     <t>Ruim</t>
   </si>
@@ -1061,7 +1061,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1129,67 +1129,7 @@
     <xf numFmtId="0" fontId="16" fillId="39" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="26" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="26" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="37" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="37" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="37" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="40" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="40" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="40" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1240,6 +1180,67 @@
     <xf numFmtId="0" fontId="0" fillId="40" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="40" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="40" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="40" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="40" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1887,7 +1888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
@@ -1914,1085 +1915,1085 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="80" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="68" t="s">
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="69" t="s">
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="70"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="91"/>
-      <c r="O1" s="92"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="72"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
-      <c r="R1" s="99"/>
+      <c r="R1" s="79"/>
       <c r="S1" s="2"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="67"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="72" t="s">
+      <c r="A2" s="80"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="73" t="s">
+      <c r="G2" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="74" t="s">
+      <c r="H2" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="72" t="s">
+      <c r="I2" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="87"/>
-      <c r="K2" s="73" t="s">
+      <c r="J2" s="67"/>
+      <c r="K2" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="L2" s="72" t="s">
+      <c r="L2" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="72" t="s">
+      <c r="M2" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="N2" s="87"/>
-      <c r="O2" s="93"/>
+      <c r="N2" s="67"/>
+      <c r="O2" s="73"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="77">
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="57">
         <v>1</v>
       </c>
-      <c r="G3" s="77">
+      <c r="G3" s="57">
         <v>1</v>
       </c>
-      <c r="H3" s="77">
+      <c r="H3" s="57">
         <v>1</v>
       </c>
-      <c r="I3" s="78" t="s">
+      <c r="I3" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="87"/>
-      <c r="K3" s="77">
+      <c r="J3" s="67"/>
+      <c r="K3" s="57">
         <v>1</v>
       </c>
-      <c r="L3" s="79" t="s">
+      <c r="L3" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="77">
+      <c r="M3" s="57">
         <v>5</v>
       </c>
-      <c r="N3" s="87"/>
-      <c r="O3" s="93"/>
+      <c r="N3" s="67"/>
+      <c r="O3" s="73"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="74" t="s">
+      <c r="A4" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="72" t="s">
+      <c r="C4" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="88"/>
-      <c r="E4" s="87"/>
-      <c r="F4" s="77">
-        <v>2</v>
-      </c>
-      <c r="G4" s="77">
-        <v>2</v>
-      </c>
-      <c r="H4" s="77">
+      <c r="D4" s="68"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="57">
+        <v>2</v>
+      </c>
+      <c r="G4" s="57">
+        <v>2</v>
+      </c>
+      <c r="H4" s="57">
         <v>1</v>
       </c>
-      <c r="I4" s="78" t="s">
+      <c r="I4" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="87"/>
-      <c r="K4" s="77">
-        <v>2</v>
-      </c>
-      <c r="L4" s="77" t="s">
+      <c r="J4" s="67"/>
+      <c r="K4" s="57">
+        <v>2</v>
+      </c>
+      <c r="L4" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="77">
+      <c r="M4" s="57">
         <v>5</v>
       </c>
-      <c r="N4" s="87"/>
-      <c r="O4" s="93"/>
+      <c r="N4" s="67"/>
+      <c r="O4" s="73"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="80">
+      <c r="A5" s="60">
         <v>1</v>
       </c>
-      <c r="B5" s="77" t="s">
+      <c r="B5" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="81" t="s">
+      <c r="C5" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="88"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="77">
+      <c r="D5" s="68"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="57">
         <v>3</v>
       </c>
-      <c r="G5" s="77">
+      <c r="G5" s="57">
         <v>3</v>
       </c>
-      <c r="H5" s="77">
+      <c r="H5" s="57">
         <v>1</v>
       </c>
-      <c r="I5" s="78" t="s">
+      <c r="I5" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="87"/>
-      <c r="K5" s="77">
+      <c r="J5" s="67"/>
+      <c r="K5" s="57">
         <v>3</v>
       </c>
-      <c r="L5" s="77" t="s">
+      <c r="L5" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="M5" s="77">
+      <c r="M5" s="57">
         <v>4</v>
       </c>
-      <c r="N5" s="87"/>
-      <c r="O5" s="93"/>
+      <c r="N5" s="67"/>
+      <c r="O5" s="73"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="77">
-        <v>2</v>
-      </c>
-      <c r="B6" s="77" t="s">
+      <c r="A6" s="57">
+        <v>2</v>
+      </c>
+      <c r="B6" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="77">
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="57">
         <v>4</v>
       </c>
-      <c r="G6" s="77">
+      <c r="G6" s="57">
         <v>1</v>
       </c>
-      <c r="H6" s="77">
-        <v>2</v>
-      </c>
-      <c r="I6" s="78" t="s">
+      <c r="H6" s="57">
+        <v>2</v>
+      </c>
+      <c r="I6" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="87"/>
-      <c r="K6" s="87"/>
-      <c r="L6" s="87"/>
-      <c r="M6" s="87"/>
-      <c r="N6" s="87"/>
-      <c r="O6" s="93"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="67"/>
+      <c r="N6" s="67"/>
+      <c r="O6" s="73"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="77">
+      <c r="A7" s="57">
         <v>3</v>
       </c>
-      <c r="B7" s="77" t="s">
+      <c r="B7" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="78" t="s">
+      <c r="C7" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="87"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="77">
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="57">
         <v>5</v>
       </c>
-      <c r="G7" s="77">
-        <v>2</v>
-      </c>
-      <c r="H7" s="77">
-        <v>2</v>
-      </c>
-      <c r="I7" s="78" t="s">
+      <c r="G7" s="57">
+        <v>2</v>
+      </c>
+      <c r="H7" s="57">
+        <v>2</v>
+      </c>
+      <c r="I7" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="87"/>
-      <c r="K7" s="87"/>
-      <c r="L7" s="87"/>
-      <c r="M7" s="87"/>
-      <c r="N7" s="87"/>
-      <c r="O7" s="93"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="67"/>
+      <c r="O7" s="73"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="94"/>
-      <c r="B8" s="87"/>
-      <c r="C8" s="87"/>
-      <c r="D8" s="87"/>
-      <c r="E8" s="87"/>
-      <c r="F8" s="77">
+      <c r="A8" s="74"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="57">
         <v>6</v>
       </c>
-      <c r="G8" s="77">
+      <c r="G8" s="57">
         <v>3</v>
       </c>
-      <c r="H8" s="77">
-        <v>2</v>
-      </c>
-      <c r="I8" s="78" t="s">
+      <c r="H8" s="57">
+        <v>2</v>
+      </c>
+      <c r="I8" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="J8" s="87"/>
-      <c r="K8" s="68" t="s">
+      <c r="J8" s="67"/>
+      <c r="K8" s="81" t="s">
         <v>52</v>
       </c>
-      <c r="L8" s="68"/>
-      <c r="M8" s="68"/>
-      <c r="N8" s="87"/>
-      <c r="O8" s="93"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="81"/>
+      <c r="N8" s="67"/>
+      <c r="O8" s="73"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="94"/>
-      <c r="B9" s="87"/>
-      <c r="C9" s="87"/>
-      <c r="D9" s="87"/>
-      <c r="E9" s="87"/>
-      <c r="F9" s="77">
+      <c r="A9" s="74"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="57">
         <v>7</v>
       </c>
-      <c r="G9" s="80">
+      <c r="G9" s="60">
         <v>1</v>
       </c>
-      <c r="H9" s="77">
+      <c r="H9" s="57">
         <v>3</v>
       </c>
-      <c r="I9" s="78" t="s">
+      <c r="I9" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="87"/>
-      <c r="K9" s="82" t="s">
+      <c r="J9" s="67"/>
+      <c r="K9" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="L9" s="72" t="s">
+      <c r="L9" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="M9" s="72" t="s">
+      <c r="M9" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="N9" s="87"/>
-      <c r="O9" s="93"/>
+      <c r="N9" s="67"/>
+      <c r="O9" s="73"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="76" t="s">
+      <c r="A10" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="76"/>
-      <c r="C10" s="76"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="87"/>
-      <c r="F10" s="77">
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="57">
         <v>8</v>
       </c>
-      <c r="G10" s="77">
-        <v>2</v>
-      </c>
-      <c r="H10" s="77">
+      <c r="G10" s="57">
+        <v>2</v>
+      </c>
+      <c r="H10" s="57">
         <v>3</v>
       </c>
-      <c r="I10" s="78" t="s">
+      <c r="I10" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="87"/>
-      <c r="K10" s="77">
+      <c r="J10" s="67"/>
+      <c r="K10" s="57">
         <v>1</v>
       </c>
-      <c r="L10" s="77" t="s">
-        <v>2</v>
-      </c>
-      <c r="M10" s="77">
+      <c r="L10" s="57" t="s">
+        <v>2</v>
+      </c>
+      <c r="M10" s="57">
         <v>11</v>
       </c>
-      <c r="N10" s="87"/>
-      <c r="O10" s="93"/>
+      <c r="N10" s="67"/>
+      <c r="O10" s="73"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="72" t="s">
+      <c r="A11" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="75" t="s">
+      <c r="B11" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="72" t="s">
+      <c r="D11" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="87"/>
-      <c r="F11" s="77">
+      <c r="E11" s="67"/>
+      <c r="F11" s="57">
         <v>9</v>
       </c>
-      <c r="G11" s="77">
+      <c r="G11" s="57">
         <v>3</v>
       </c>
-      <c r="H11" s="77">
+      <c r="H11" s="57">
         <v>3</v>
       </c>
-      <c r="I11" s="78" t="s">
+      <c r="I11" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="J11" s="87"/>
-      <c r="K11" s="77">
-        <v>2</v>
-      </c>
-      <c r="L11" s="77" t="s">
+      <c r="J11" s="67"/>
+      <c r="K11" s="57">
+        <v>2</v>
+      </c>
+      <c r="L11" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="M11" s="77">
+      <c r="M11" s="57">
         <v>3</v>
       </c>
-      <c r="N11" s="87"/>
-      <c r="O11" s="93"/>
+      <c r="N11" s="67"/>
+      <c r="O11" s="73"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="77">
+      <c r="A12" s="57">
         <v>1</v>
       </c>
-      <c r="B12" s="77">
+      <c r="B12" s="57">
         <v>1</v>
       </c>
-      <c r="C12" s="77">
+      <c r="C12" s="57">
         <v>1</v>
       </c>
-      <c r="D12" s="85" t="s">
+      <c r="D12" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="87"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="87"/>
-      <c r="H12" s="88"/>
-      <c r="I12" s="87"/>
-      <c r="J12" s="87"/>
-      <c r="K12" s="87"/>
-      <c r="L12" s="87"/>
-      <c r="M12" s="87"/>
-      <c r="N12" s="87"/>
-      <c r="O12" s="93"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="67"/>
+      <c r="N12" s="67"/>
+      <c r="O12" s="73"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="77">
-        <v>2</v>
-      </c>
-      <c r="B13" s="77">
+      <c r="A13" s="57">
+        <v>2</v>
+      </c>
+      <c r="B13" s="57">
         <v>1</v>
       </c>
-      <c r="C13" s="77">
-        <v>2</v>
-      </c>
-      <c r="D13" s="85" t="s">
+      <c r="C13" s="57">
+        <v>2</v>
+      </c>
+      <c r="D13" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="87"/>
-      <c r="F13" s="87"/>
-      <c r="G13" s="87"/>
-      <c r="H13" s="88"/>
-      <c r="I13" s="87"/>
-      <c r="J13" s="87"/>
-      <c r="K13" s="87"/>
-      <c r="L13" s="87"/>
-      <c r="M13" s="87"/>
-      <c r="N13" s="87"/>
-      <c r="O13" s="93"/>
+      <c r="E13" s="67"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="67"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="67"/>
+      <c r="O13" s="73"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="77">
+      <c r="A14" s="57">
         <v>3</v>
       </c>
-      <c r="B14" s="77">
+      <c r="B14" s="57">
         <v>1</v>
       </c>
-      <c r="C14" s="77">
+      <c r="C14" s="57">
         <v>3</v>
       </c>
-      <c r="D14" s="85" t="s">
+      <c r="D14" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="87"/>
-      <c r="F14" s="68" t="s">
+      <c r="E14" s="67"/>
+      <c r="F14" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="68"/>
-      <c r="H14" s="68"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="87"/>
-      <c r="K14" s="68" t="s">
+      <c r="G14" s="81"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="L14" s="68"/>
-      <c r="M14" s="68"/>
-      <c r="N14" s="87"/>
-      <c r="O14" s="93"/>
+      <c r="L14" s="81"/>
+      <c r="M14" s="81"/>
+      <c r="N14" s="67"/>
+      <c r="O14" s="73"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="77">
+      <c r="A15" s="57">
         <v>4</v>
       </c>
-      <c r="B15" s="77">
-        <v>2</v>
-      </c>
-      <c r="C15" s="77">
+      <c r="B15" s="57">
+        <v>2</v>
+      </c>
+      <c r="C15" s="57">
         <v>1</v>
       </c>
-      <c r="D15" s="85" t="s">
+      <c r="D15" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="87"/>
-      <c r="F15" s="72" t="s">
+      <c r="E15" s="67"/>
+      <c r="F15" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="82" t="s">
+      <c r="G15" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="H15" s="74" t="s">
+      <c r="H15" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="I15" s="72" t="s">
+      <c r="I15" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="J15" s="87"/>
-      <c r="K15" s="75" t="s">
+      <c r="J15" s="67"/>
+      <c r="K15" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="L15" s="72" t="s">
+      <c r="L15" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="M15" s="72" t="s">
+      <c r="M15" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="N15" s="87"/>
-      <c r="O15" s="93"/>
+      <c r="N15" s="67"/>
+      <c r="O15" s="73"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="77">
+      <c r="A16" s="57">
         <v>5</v>
       </c>
-      <c r="B16" s="77">
-        <v>2</v>
-      </c>
-      <c r="C16" s="77">
-        <v>2</v>
-      </c>
-      <c r="D16" s="85" t="s">
+      <c r="B16" s="57">
+        <v>2</v>
+      </c>
+      <c r="C16" s="57">
+        <v>2</v>
+      </c>
+      <c r="D16" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="E16" s="87"/>
-      <c r="F16" s="77">
+      <c r="E16" s="67"/>
+      <c r="F16" s="57">
         <v>1</v>
       </c>
-      <c r="G16" s="77">
+      <c r="G16" s="57">
         <v>1</v>
       </c>
-      <c r="H16" s="86" t="s">
+      <c r="H16" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="86" t="s">
+      <c r="I16" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="J16" s="87"/>
-      <c r="K16" s="77">
+      <c r="J16" s="67"/>
+      <c r="K16" s="57">
         <v>1</v>
       </c>
-      <c r="L16" s="77" t="s">
+      <c r="L16" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="M16" s="77">
+      <c r="M16" s="57">
         <v>7</v>
       </c>
-      <c r="N16" s="87"/>
-      <c r="O16" s="93"/>
+      <c r="N16" s="67"/>
+      <c r="O16" s="73"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="77">
+      <c r="A17" s="57">
         <v>6</v>
       </c>
-      <c r="B17" s="77">
-        <v>2</v>
-      </c>
-      <c r="C17" s="77">
+      <c r="B17" s="57">
+        <v>2</v>
+      </c>
+      <c r="C17" s="57">
         <v>3</v>
       </c>
-      <c r="D17" s="85" t="s">
+      <c r="D17" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="87"/>
-      <c r="F17" s="77">
-        <v>2</v>
-      </c>
-      <c r="G17" s="77">
+      <c r="E17" s="67"/>
+      <c r="F17" s="57">
+        <v>2</v>
+      </c>
+      <c r="G17" s="57">
         <v>1</v>
       </c>
-      <c r="H17" s="86" t="s">
+      <c r="H17" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="I17" s="86" t="s">
+      <c r="I17" s="66" t="s">
         <v>47</v>
       </c>
-      <c r="J17" s="87"/>
-      <c r="K17" s="77">
-        <v>2</v>
-      </c>
-      <c r="L17" s="77" t="s">
+      <c r="J17" s="67"/>
+      <c r="K17" s="57">
+        <v>2</v>
+      </c>
+      <c r="L17" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="M17" s="77">
+      <c r="M17" s="57">
         <v>7</v>
       </c>
-      <c r="N17" s="87"/>
-      <c r="O17" s="93"/>
+      <c r="N17" s="67"/>
+      <c r="O17" s="73"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="94"/>
-      <c r="B18" s="87"/>
-      <c r="C18" s="87"/>
-      <c r="D18" s="87"/>
-      <c r="E18" s="87"/>
-      <c r="F18" s="77">
+      <c r="A18" s="74"/>
+      <c r="B18" s="67"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="57">
         <v>3</v>
       </c>
-      <c r="G18" s="77">
+      <c r="G18" s="57">
         <v>1</v>
       </c>
-      <c r="H18" s="86" t="s">
+      <c r="H18" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="I18" s="86" t="s">
+      <c r="I18" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="J18" s="87"/>
-      <c r="K18" s="87"/>
-      <c r="L18" s="87"/>
-      <c r="M18" s="87"/>
-      <c r="N18" s="87"/>
-      <c r="O18" s="93"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="67"/>
+      <c r="L18" s="67"/>
+      <c r="M18" s="67"/>
+      <c r="N18" s="67"/>
+      <c r="O18" s="73"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="94"/>
-      <c r="B19" s="87"/>
-      <c r="C19" s="87"/>
-      <c r="D19" s="87"/>
-      <c r="E19" s="95"/>
-      <c r="F19" s="77">
+      <c r="A19" s="74"/>
+      <c r="B19" s="67"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="75"/>
+      <c r="F19" s="57">
         <v>4</v>
       </c>
-      <c r="G19" s="77">
-        <v>2</v>
-      </c>
-      <c r="H19" s="86" t="s">
+      <c r="G19" s="57">
+        <v>2</v>
+      </c>
+      <c r="H19" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="I19" s="86" t="s">
+      <c r="I19" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="J19" s="87"/>
-      <c r="K19" s="87"/>
-      <c r="L19" s="87"/>
-      <c r="M19" s="87"/>
-      <c r="N19" s="87"/>
-      <c r="O19" s="93"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="67"/>
+      <c r="L19" s="67"/>
+      <c r="M19" s="67"/>
+      <c r="N19" s="67"/>
+      <c r="O19" s="73"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="76" t="s">
+      <c r="A20" s="56" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="76"/>
-      <c r="C20" s="76"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="95"/>
-      <c r="F20" s="77">
+      <c r="B20" s="56"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="75"/>
+      <c r="F20" s="57">
         <v>5</v>
       </c>
-      <c r="G20" s="77">
-        <v>2</v>
-      </c>
-      <c r="H20" s="86" t="s">
+      <c r="G20" s="57">
+        <v>2</v>
+      </c>
+      <c r="H20" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="I20" s="86" t="s">
+      <c r="I20" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="J20" s="87"/>
-      <c r="K20" s="68" t="s">
+      <c r="J20" s="67"/>
+      <c r="K20" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="L20" s="68"/>
-      <c r="M20" s="68"/>
-      <c r="N20" s="68"/>
-      <c r="O20" s="93"/>
+      <c r="L20" s="81"/>
+      <c r="M20" s="81"/>
+      <c r="N20" s="81"/>
+      <c r="O20" s="73"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="89" t="s">
+      <c r="A21" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="83" t="s">
+      <c r="B21" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="74" t="s">
+      <c r="C21" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="89" t="s">
+      <c r="D21" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="95"/>
-      <c r="F21" s="77">
+      <c r="E21" s="75"/>
+      <c r="F21" s="57">
         <v>6</v>
       </c>
-      <c r="G21" s="77">
-        <v>2</v>
-      </c>
-      <c r="H21" s="86" t="s">
+      <c r="G21" s="57">
+        <v>2</v>
+      </c>
+      <c r="H21" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="86" t="s">
+      <c r="I21" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="J21" s="87"/>
-      <c r="K21" s="83" t="s">
+      <c r="J21" s="67"/>
+      <c r="K21" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="L21" s="72" t="s">
+      <c r="L21" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="M21" s="72" t="s">
+      <c r="M21" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="N21" s="72" t="s">
+      <c r="N21" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="O21" s="93"/>
+      <c r="O21" s="73"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="77">
+      <c r="A22" s="57">
         <v>1</v>
       </c>
-      <c r="B22" s="77">
+      <c r="B22" s="57">
         <v>1</v>
       </c>
-      <c r="C22" s="77">
+      <c r="C22" s="57">
         <v>1</v>
       </c>
-      <c r="D22" s="85" t="s">
+      <c r="D22" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="95"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="87"/>
-      <c r="H22" s="88"/>
-      <c r="I22" s="87"/>
-      <c r="J22" s="87"/>
-      <c r="K22" s="77">
+      <c r="E22" s="75"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="68"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="67"/>
+      <c r="K22" s="57">
         <v>1</v>
       </c>
-      <c r="L22" s="77">
+      <c r="L22" s="57">
         <v>0</v>
       </c>
-      <c r="M22" s="84">
+      <c r="M22" s="64">
         <v>15000</v>
       </c>
-      <c r="N22" s="77">
+      <c r="N22" s="57">
         <v>3</v>
       </c>
-      <c r="O22" s="93"/>
+      <c r="O22" s="73"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="77">
-        <v>2</v>
-      </c>
-      <c r="B23" s="77">
-        <v>2</v>
-      </c>
-      <c r="C23" s="77">
+      <c r="A23" s="57">
+        <v>2</v>
+      </c>
+      <c r="B23" s="57">
+        <v>2</v>
+      </c>
+      <c r="C23" s="57">
         <v>1</v>
       </c>
-      <c r="D23" s="85" t="s">
+      <c r="D23" s="65" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="95"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="87"/>
-      <c r="H23" s="88"/>
-      <c r="I23" s="87"/>
-      <c r="J23" s="87"/>
-      <c r="K23" s="77">
-        <v>2</v>
-      </c>
-      <c r="L23" s="84">
+      <c r="E23" s="75"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="67"/>
+      <c r="K23" s="57">
+        <v>2</v>
+      </c>
+      <c r="L23" s="64">
         <v>15000</v>
       </c>
-      <c r="M23" s="84">
+      <c r="M23" s="64">
         <v>35000</v>
       </c>
-      <c r="N23" s="77">
+      <c r="N23" s="57">
         <v>4</v>
       </c>
-      <c r="O23" s="93"/>
+      <c r="O23" s="73"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="77">
+      <c r="A24" s="57">
         <v>3</v>
       </c>
-      <c r="B24" s="77">
+      <c r="B24" s="57">
         <v>3</v>
       </c>
-      <c r="C24" s="77">
+      <c r="C24" s="57">
         <v>1</v>
       </c>
-      <c r="D24" s="85" t="s">
+      <c r="D24" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="E24" s="95"/>
-      <c r="F24" s="87"/>
-      <c r="G24" s="87"/>
-      <c r="H24" s="87"/>
-      <c r="I24" s="87"/>
-      <c r="J24" s="87"/>
-      <c r="K24" s="77">
+      <c r="E24" s="75"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="67"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="57">
         <v>3</v>
       </c>
-      <c r="L24" s="84">
+      <c r="L24" s="64">
         <v>35000</v>
       </c>
-      <c r="M24" s="84">
+      <c r="M24" s="64">
         <v>35000</v>
       </c>
-      <c r="N24" s="77">
+      <c r="N24" s="57">
         <v>7</v>
       </c>
-      <c r="O24" s="93"/>
+      <c r="O24" s="73"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
       <c r="S24" s="2"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="77">
+      <c r="A25" s="57">
         <v>4</v>
       </c>
-      <c r="B25" s="77">
+      <c r="B25" s="57">
         <v>1</v>
       </c>
-      <c r="C25" s="77">
-        <v>2</v>
-      </c>
-      <c r="D25" s="85" t="s">
+      <c r="C25" s="57">
+        <v>2</v>
+      </c>
+      <c r="D25" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="87"/>
-      <c r="F25" s="87"/>
-      <c r="G25" s="87"/>
-      <c r="H25" s="87"/>
-      <c r="I25" s="87"/>
-      <c r="J25" s="87"/>
-      <c r="K25" s="87"/>
-      <c r="L25" s="87"/>
-      <c r="M25" s="87"/>
-      <c r="N25" s="87"/>
-      <c r="O25" s="93"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="67"/>
+      <c r="I25" s="67"/>
+      <c r="J25" s="67"/>
+      <c r="K25" s="67"/>
+      <c r="L25" s="67"/>
+      <c r="M25" s="67"/>
+      <c r="N25" s="67"/>
+      <c r="O25" s="73"/>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="77">
+      <c r="A26" s="57">
         <v>5</v>
       </c>
-      <c r="B26" s="77">
-        <v>2</v>
-      </c>
-      <c r="C26" s="77">
-        <v>2</v>
-      </c>
-      <c r="D26" s="85" t="s">
+      <c r="B26" s="57">
+        <v>2</v>
+      </c>
+      <c r="C26" s="57">
+        <v>2</v>
+      </c>
+      <c r="D26" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="87"/>
-      <c r="F26" s="87"/>
-      <c r="G26" s="87"/>
-      <c r="H26" s="87"/>
-      <c r="I26" s="87"/>
-      <c r="J26" s="87"/>
-      <c r="K26" s="87"/>
-      <c r="L26" s="87"/>
-      <c r="M26" s="87"/>
-      <c r="N26" s="87"/>
-      <c r="O26" s="93"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="67"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="67"/>
+      <c r="J26" s="67"/>
+      <c r="K26" s="67"/>
+      <c r="L26" s="67"/>
+      <c r="M26" s="67"/>
+      <c r="N26" s="67"/>
+      <c r="O26" s="73"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
       <c r="S26" s="2"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="77">
+      <c r="A27" s="57">
         <v>6</v>
       </c>
-      <c r="B27" s="77">
+      <c r="B27" s="57">
         <v>3</v>
       </c>
-      <c r="C27" s="77">
-        <v>2</v>
-      </c>
-      <c r="D27" s="85" t="s">
+      <c r="C27" s="57">
+        <v>2</v>
+      </c>
+      <c r="D27" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="87"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
-      <c r="H27" s="87"/>
-      <c r="I27" s="87"/>
-      <c r="J27" s="87"/>
-      <c r="K27" s="87"/>
-      <c r="L27" s="87"/>
-      <c r="M27" s="87"/>
-      <c r="N27" s="87"/>
-      <c r="O27" s="93"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="67"/>
+      <c r="I27" s="67"/>
+      <c r="J27" s="67"/>
+      <c r="K27" s="67"/>
+      <c r="L27" s="67"/>
+      <c r="M27" s="67"/>
+      <c r="N27" s="67"/>
+      <c r="O27" s="73"/>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A28" s="77">
+      <c r="A28" s="57">
         <v>7</v>
       </c>
-      <c r="B28" s="77">
+      <c r="B28" s="57">
         <v>1</v>
       </c>
-      <c r="C28" s="77">
+      <c r="C28" s="57">
         <v>3</v>
       </c>
-      <c r="D28" s="85" t="s">
+      <c r="D28" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="E28" s="87"/>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87"/>
-      <c r="H28" s="87"/>
-      <c r="I28" s="87"/>
-      <c r="J28" s="87"/>
-      <c r="K28" s="87"/>
-      <c r="L28" s="87"/>
-      <c r="M28" s="87"/>
-      <c r="N28" s="87"/>
-      <c r="O28" s="93"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="67"/>
+      <c r="I28" s="67"/>
+      <c r="J28" s="67"/>
+      <c r="K28" s="67"/>
+      <c r="L28" s="67"/>
+      <c r="M28" s="67"/>
+      <c r="N28" s="67"/>
+      <c r="O28" s="73"/>
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
       <c r="S28" s="2"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A29" s="77">
+      <c r="A29" s="57">
         <v>8</v>
       </c>
-      <c r="B29" s="77">
-        <v>2</v>
-      </c>
-      <c r="C29" s="77">
+      <c r="B29" s="57">
+        <v>2</v>
+      </c>
+      <c r="C29" s="57">
         <v>3</v>
       </c>
-      <c r="D29" s="85" t="s">
+      <c r="D29" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="87"/>
-      <c r="F29" s="87"/>
-      <c r="G29" s="87"/>
-      <c r="H29" s="87"/>
-      <c r="I29" s="87"/>
-      <c r="J29" s="87"/>
-      <c r="K29" s="87"/>
-      <c r="L29" s="87"/>
-      <c r="M29" s="87"/>
-      <c r="N29" s="87"/>
-      <c r="O29" s="93"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="67"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="67"/>
+      <c r="J29" s="67"/>
+      <c r="K29" s="67"/>
+      <c r="L29" s="67"/>
+      <c r="M29" s="67"/>
+      <c r="N29" s="67"/>
+      <c r="O29" s="73"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
       <c r="S29" s="2"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="77">
+      <c r="A30" s="57">
         <v>9</v>
       </c>
-      <c r="B30" s="77">
+      <c r="B30" s="57">
         <v>3</v>
       </c>
-      <c r="C30" s="77">
+      <c r="C30" s="57">
         <v>3</v>
       </c>
-      <c r="D30" s="85" t="s">
+      <c r="D30" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="E30" s="87"/>
-      <c r="F30" s="87"/>
-      <c r="G30" s="87"/>
-      <c r="H30" s="87"/>
-      <c r="I30" s="87"/>
-      <c r="J30" s="87"/>
-      <c r="K30" s="87"/>
-      <c r="L30" s="87"/>
-      <c r="M30" s="87"/>
-      <c r="N30" s="87"/>
-      <c r="O30" s="93"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="67"/>
+      <c r="I30" s="67"/>
+      <c r="J30" s="67"/>
+      <c r="K30" s="67"/>
+      <c r="L30" s="67"/>
+      <c r="M30" s="67"/>
+      <c r="N30" s="67"/>
+      <c r="O30" s="73"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
       <c r="S30" s="2"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="94"/>
-      <c r="B31" s="87"/>
-      <c r="C31" s="87"/>
-      <c r="D31" s="87"/>
-      <c r="E31" s="87"/>
-      <c r="F31" s="87"/>
-      <c r="G31" s="87"/>
-      <c r="H31" s="90"/>
-      <c r="I31" s="87"/>
-      <c r="J31" s="87"/>
-      <c r="K31" s="87"/>
-      <c r="L31" s="87"/>
-      <c r="M31" s="87"/>
-      <c r="N31" s="87"/>
-      <c r="O31" s="93"/>
+      <c r="A31" s="74"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="67"/>
+      <c r="D31" s="67"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="67"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="70"/>
+      <c r="I31" s="67"/>
+      <c r="J31" s="67"/>
+      <c r="K31" s="67"/>
+      <c r="L31" s="67"/>
+      <c r="M31" s="67"/>
+      <c r="N31" s="67"/>
+      <c r="O31" s="73"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
       <c r="S31" s="2"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A32" s="96"/>
-      <c r="B32" s="97"/>
-      <c r="C32" s="97"/>
-      <c r="D32" s="97"/>
-      <c r="E32" s="97"/>
-      <c r="F32" s="97"/>
-      <c r="G32" s="97"/>
-      <c r="H32" s="97"/>
-      <c r="I32" s="97"/>
-      <c r="J32" s="97"/>
-      <c r="K32" s="97"/>
-      <c r="L32" s="97"/>
-      <c r="M32" s="97"/>
-      <c r="N32" s="97"/>
-      <c r="O32" s="98"/>
+      <c r="A32" s="76"/>
+      <c r="B32" s="77"/>
+      <c r="C32" s="77"/>
+      <c r="D32" s="77"/>
+      <c r="E32" s="77"/>
+      <c r="F32" s="77"/>
+      <c r="G32" s="77"/>
+      <c r="H32" s="77"/>
+      <c r="I32" s="77"/>
+      <c r="J32" s="77"/>
+      <c r="K32" s="77"/>
+      <c r="L32" s="77"/>
+      <c r="M32" s="77"/>
+      <c r="N32" s="77"/>
+      <c r="O32" s="78"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
       <c r="S32" s="2"/>
-      <c r="T32" s="66"/>
+      <c r="T32" s="51"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
@@ -3014,7 +3015,7 @@
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
       <c r="S33" s="2"/>
-      <c r="T33" s="66"/>
+      <c r="T33" s="51"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
@@ -3036,7 +3037,7 @@
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
       <c r="S34" s="2"/>
-      <c r="T34" s="66"/>
+      <c r="T34" s="51"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
@@ -3058,61 +3059,61 @@
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
       <c r="S35" s="2"/>
-      <c r="T35" s="66"/>
+      <c r="T35" s="51"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A36" s="66"/>
-      <c r="B36" s="66"/>
-      <c r="C36" s="66"/>
-      <c r="D36" s="66"/>
-      <c r="E36" s="66"/>
-      <c r="F36" s="66"/>
-      <c r="G36" s="66"/>
-      <c r="H36" s="66"/>
-      <c r="I36" s="66"/>
-      <c r="J36" s="66"/>
-      <c r="K36" s="66"/>
-      <c r="L36" s="66"/>
-      <c r="M36" s="66"/>
-      <c r="N36" s="66"/>
-      <c r="O36" s="66"/>
-      <c r="P36" s="66"/>
-      <c r="Q36" s="66"/>
-      <c r="R36" s="66"/>
-      <c r="S36" s="66"/>
-      <c r="T36" s="66"/>
+      <c r="A36" s="51"/>
+      <c r="B36" s="51"/>
+      <c r="C36" s="51"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="51"/>
+      <c r="H36" s="51"/>
+      <c r="I36" s="51"/>
+      <c r="J36" s="51"/>
+      <c r="K36" s="51"/>
+      <c r="L36" s="51"/>
+      <c r="M36" s="51"/>
+      <c r="N36" s="51"/>
+      <c r="O36" s="51"/>
+      <c r="P36" s="51"/>
+      <c r="Q36" s="51"/>
+      <c r="R36" s="51"/>
+      <c r="S36" s="51"/>
+      <c r="T36" s="51"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A37" s="66"/>
-      <c r="B37" s="66"/>
-      <c r="C37" s="66"/>
-      <c r="D37" s="66"/>
-      <c r="E37" s="66"/>
-      <c r="F37" s="66"/>
-      <c r="G37" s="66"/>
-      <c r="H37" s="66"/>
-      <c r="I37" s="66"/>
-      <c r="J37" s="66"/>
-      <c r="K37" s="66"/>
-      <c r="L37" s="66"/>
-      <c r="M37" s="66"/>
-      <c r="N37" s="66"/>
-      <c r="O37" s="66"/>
-      <c r="P37" s="66"/>
-      <c r="Q37" s="66"/>
-      <c r="R37" s="66"/>
-      <c r="S37" s="66"/>
-      <c r="T37" s="66"/>
+      <c r="A37" s="51"/>
+      <c r="B37" s="51"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="51"/>
+      <c r="I37" s="51"/>
+      <c r="J37" s="51"/>
+      <c r="K37" s="51"/>
+      <c r="L37" s="51"/>
+      <c r="M37" s="51"/>
+      <c r="N37" s="51"/>
+      <c r="O37" s="51"/>
+      <c r="P37" s="51"/>
+      <c r="Q37" s="51"/>
+      <c r="R37" s="51"/>
+      <c r="S37" s="51"/>
+      <c r="T37" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="F1:I1"/>
     <mergeCell ref="A1:C2"/>
     <mergeCell ref="K14:M14"/>
     <mergeCell ref="F14:I14"/>
     <mergeCell ref="K8:M8"/>
     <mergeCell ref="K1:M1"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="F1:I1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3123,8 +3124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD1FCB17-DE8B-4353-BED0-F48067874117}">
   <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3140,10 +3141,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="89" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="61"/>
+      <c r="B1" s="89"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -3199,14 +3200,14 @@
       <c r="S6" s="8"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="91" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="64"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="65"/>
+      <c r="B7" s="92"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="93"/>
       <c r="G7" s="26" t="s">
         <v>73</v>
       </c>
@@ -3344,7 +3345,7 @@
       </c>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
+      <c r="L10" s="100"/>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
       <c r="O10" s="8"/>
@@ -3356,12 +3357,12 @@
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
-      <c r="C11" s="59" t="s">
+      <c r="C11" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
+      <c r="D11" s="94"/>
+      <c r="E11" s="94"/>
+      <c r="F11" s="94"/>
       <c r="G11" s="25">
         <f>SUM(G8:G10)</f>
         <v>6.4656084656084661E-2</v>
@@ -3399,15 +3400,15 @@
       <c r="S12" s="8"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="62" t="s">
+      <c r="A13" s="90" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="62"/>
+      <c r="B13" s="90"/>
       <c r="C13" s="13"/>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="60" t="s">
+      <c r="G13" s="85" t="s">
         <v>75</v>
       </c>
       <c r="H13" s="8"/>
@@ -3434,7 +3435,7 @@
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
-      <c r="G14" s="60"/>
+      <c r="G14" s="85"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
@@ -3459,7 +3460,7 @@
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
-      <c r="G15" s="60"/>
+      <c r="G15" s="85"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
@@ -3484,7 +3485,7 @@
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
-      <c r="G16" s="60"/>
+      <c r="G16" s="85"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
@@ -3509,7 +3510,7 @@
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
-      <c r="G17" s="60"/>
+      <c r="G17" s="85"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
@@ -3545,14 +3546,14 @@
       <c r="S18" s="8"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="56" t="s">
+      <c r="A19" s="86" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="58"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="87"/>
+      <c r="D19" s="87"/>
+      <c r="E19" s="87"/>
+      <c r="F19" s="88"/>
       <c r="G19" s="26" t="s">
         <v>73</v>
       </c>
@@ -3699,12 +3700,12 @@
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
-      <c r="C23" s="59" t="s">
+      <c r="C23" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="59"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="59"/>
+      <c r="D23" s="94"/>
+      <c r="E23" s="94"/>
+      <c r="F23" s="94"/>
       <c r="G23" s="15">
         <f>SUM(G20:G22)</f>
         <v>0</v>
@@ -3744,12 +3745,12 @@
       <c r="S24" s="8"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="51" t="s">
+      <c r="A25" s="95" t="s">
         <v>81</v>
       </c>
-      <c r="B25" s="51"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="51"/>
+      <c r="B25" s="95"/>
+      <c r="C25" s="95"/>
+      <c r="D25" s="95"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
@@ -3763,14 +3764,14 @@
       <c r="S25" s="8"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="56" t="s">
+      <c r="A26" s="86" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="58"/>
+      <c r="B26" s="87"/>
+      <c r="C26" s="87"/>
+      <c r="D26" s="87"/>
+      <c r="E26" s="87"/>
+      <c r="F26" s="88"/>
       <c r="G26" s="26" t="s">
         <v>73</v>
       </c>
@@ -3900,12 +3901,12 @@
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
-      <c r="C30" s="52" t="s">
+      <c r="C30" s="96" t="s">
         <v>26</v>
       </c>
-      <c r="D30" s="53"/>
-      <c r="E30" s="53"/>
-      <c r="F30" s="54"/>
+      <c r="D30" s="97"/>
+      <c r="E30" s="97"/>
+      <c r="F30" s="98"/>
       <c r="G30" s="15">
         <f>SUM(G27:G29)</f>
         <v>7.3468375445416255E-3</v>
@@ -3913,18 +3914,22 @@
       <c r="H30" s="8"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="55" t="s">
+      <c r="A32" s="99" t="s">
         <v>87</v>
       </c>
-      <c r="B32" s="55"/>
-      <c r="C32" s="55"/>
-      <c r="D32" s="55"/>
-      <c r="E32" s="55"/>
-      <c r="F32" s="55"/>
-      <c r="G32" s="55"/>
+      <c r="B32" s="99"/>
+      <c r="C32" s="99"/>
+      <c r="D32" s="99"/>
+      <c r="E32" s="99"/>
+      <c r="F32" s="99"/>
+      <c r="G32" s="99"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="C23:F23"/>
     <mergeCell ref="G13:G17"/>
     <mergeCell ref="A26:F26"/>
     <mergeCell ref="A1:B1"/>
@@ -3932,10 +3937,6 @@
     <mergeCell ref="A7:F7"/>
     <mergeCell ref="C11:F11"/>
     <mergeCell ref="A25:D25"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="C23:F23"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>